<commit_message>
fixed reply part and in data obs_ID 93: reaply from 'n ' to 'n'
</commit_message>
<xml_diff>
--- a/Data/observations.xlsx
+++ b/Data/observations.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinbulla/Dropbox/Science/MS/Exchanges_SESA/Analyses/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EA14EF-A7AB-2C43-9C9C-62E4A851003E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="540" windowWidth="10230" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exchange_behavior_DT_2017-02-27" sheetId="1" r:id="rId1"/>
@@ -17,14 +23,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>muck</author>
     <author>Daniela</author>
     <author>Daniela Tritscher</author>
   </authors>
   <commentList>
-    <comment ref="U14" authorId="0">
+    <comment ref="U14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F47" authorId="1">
+    <comment ref="F47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R47" authorId="1">
+    <comment ref="R47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA47" authorId="1">
+    <comment ref="AA47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB47" authorId="1">
+    <comment ref="AB47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC47" authorId="1">
+    <comment ref="AC47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX47" authorId="1">
+    <comment ref="AX47" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P48" authorId="2">
+    <comment ref="P48" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P49" authorId="2">
+    <comment ref="P49" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="1">
+    <comment ref="A50" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -264,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F50" authorId="2">
+    <comment ref="F50" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -288,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H50" authorId="2">
+    <comment ref="H50" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -312,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL50" authorId="2">
+    <comment ref="AL50" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -336,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT50" authorId="2">
+    <comment ref="AT50" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -360,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H51" authorId="2">
+    <comment ref="H51" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -384,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y60" authorId="0">
+    <comment ref="Y60" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -408,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P71" authorId="2">
+    <comment ref="P71" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -432,7 +438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P72" authorId="2">
+    <comment ref="P72" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -456,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P73" authorId="2">
+    <comment ref="P73" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -480,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P74" authorId="2">
+    <comment ref="P74" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -504,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P75" authorId="2">
+    <comment ref="P75" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -528,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z75" authorId="0">
+    <comment ref="Z75" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -552,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P76" authorId="2">
+    <comment ref="P76" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -576,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P77" authorId="2">
+    <comment ref="P77" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -600,7 +606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P78" authorId="2">
+    <comment ref="P78" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -624,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P79" authorId="2">
+    <comment ref="P79" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -648,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P80" authorId="2">
+    <comment ref="P80" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -672,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P81" authorId="2">
+    <comment ref="P81" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -696,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S85" authorId="0">
+    <comment ref="S85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -720,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T97" authorId="0">
+    <comment ref="T97" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -744,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O104" authorId="2">
+    <comment ref="O104" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -768,7 +774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O105" authorId="2">
+    <comment ref="O105" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -792,7 +798,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U105" authorId="1">
+    <comment ref="U105" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -816,7 +822,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O106" authorId="2">
+    <comment ref="O106" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -840,7 +846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O107" authorId="2">
+    <comment ref="O107" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -864,7 +870,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O108" authorId="2">
+    <comment ref="O108" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -888,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O109" authorId="2">
+    <comment ref="O109" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -912,7 +918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P110" authorId="2">
+    <comment ref="P110" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -936,7 +942,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P111" authorId="2">
+    <comment ref="P111" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -960,7 +966,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P112" authorId="2">
+    <comment ref="P112" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -984,7 +990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P113" authorId="2">
+    <comment ref="P113" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -1008,7 +1014,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P114" authorId="2">
+    <comment ref="P114" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1038,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P115" authorId="2">
+    <comment ref="P115" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1062,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P116" authorId="2">
+    <comment ref="P116" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -1080,7 +1086,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P117" authorId="2">
+    <comment ref="P117" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -1104,7 +1110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P118" authorId="2">
+    <comment ref="P118" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P119" authorId="2">
+    <comment ref="P119" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -1152,7 +1158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P120" authorId="2">
+    <comment ref="P120" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
       <text>
         <r>
           <rPr>
@@ -1176,7 +1182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P121" authorId="2">
+    <comment ref="P121" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
       <text>
         <r>
           <rPr>
@@ -1200,7 +1206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P122" authorId="2">
+    <comment ref="P122" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -1224,7 +1230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P123" authorId="2">
+    <comment ref="P123" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000033000000}">
       <text>
         <r>
           <rPr>
@@ -1248,7 +1254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P124" authorId="2">
+    <comment ref="P124" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000034000000}">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P125" authorId="2">
+    <comment ref="P125" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000035000000}">
       <text>
         <r>
           <rPr>
@@ -1296,7 +1302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W129" authorId="0">
+    <comment ref="W129" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000036000000}">
       <text>
         <r>
           <rPr>
@@ -1320,7 +1326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z129" authorId="0">
+    <comment ref="Z129" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000037000000}">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S139" authorId="0">
+    <comment ref="S139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000038000000}">
       <text>
         <r>
           <rPr>
@@ -1368,7 +1374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T140" authorId="0">
+    <comment ref="T140" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000039000000}">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P145" authorId="2">
+    <comment ref="P145" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -1416,7 +1422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P146" authorId="2">
+    <comment ref="P146" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -1440,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P147" authorId="2">
+    <comment ref="P147" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P148" authorId="2">
+    <comment ref="P148" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -1488,7 +1494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P149" authorId="2">
+    <comment ref="P149" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -1512,7 +1518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P150" authorId="2">
+    <comment ref="P150" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P151" authorId="2">
+    <comment ref="P151" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000040000000}">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P152" authorId="2">
+    <comment ref="P152" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000041000000}">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P153" authorId="2">
+    <comment ref="P153" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000042000000}">
       <text>
         <r>
           <rPr>
@@ -1608,7 +1614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y153" authorId="0">
+    <comment ref="Y153" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000043000000}">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P154" authorId="2">
+    <comment ref="P154" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000044000000}">
       <text>
         <r>
           <rPr>
@@ -1656,7 +1662,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R154" authorId="0">
+    <comment ref="R154" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000045000000}">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z154" authorId="0">
+    <comment ref="Z154" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000046000000}">
       <text>
         <r>
           <rPr>
@@ -1704,7 +1710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P155" authorId="2">
+    <comment ref="P155" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000047000000}">
       <text>
         <r>
           <rPr>
@@ -1728,7 +1734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P159" authorId="2">
+    <comment ref="P159" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000048000000}">
       <text>
         <r>
           <rPr>
@@ -1752,7 +1758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P160" authorId="2">
+    <comment ref="P160" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000049000000}">
       <text>
         <r>
           <rPr>
@@ -1776,7 +1782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A163" authorId="1">
+    <comment ref="A163" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -1800,7 +1806,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P164" authorId="2">
+    <comment ref="P164" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1830,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ164" authorId="0">
+    <comment ref="AQ164" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -1848,7 +1854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P165" authorId="2">
+    <comment ref="P165" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -1872,7 +1878,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P166" authorId="2">
+    <comment ref="P166" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004E000000}">
       <text>
         <r>
           <rPr>
@@ -1896,7 +1902,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R166" authorId="2">
+    <comment ref="R166" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004F000000}">
       <text>
         <r>
           <rPr>
@@ -1920,7 +1926,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P167" authorId="2">
+    <comment ref="P167" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000050000000}">
       <text>
         <r>
           <rPr>
@@ -1944,7 +1950,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P168" authorId="2">
+    <comment ref="P168" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000051000000}">
       <text>
         <r>
           <rPr>
@@ -1968,7 +1974,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P169" authorId="2">
+    <comment ref="P169" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000052000000}">
       <text>
         <r>
           <rPr>
@@ -1992,7 +1998,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P170" authorId="2">
+    <comment ref="P170" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000053000000}">
       <text>
         <r>
           <rPr>
@@ -2016,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P171" authorId="2">
+    <comment ref="P171" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000054000000}">
       <text>
         <r>
           <rPr>
@@ -2040,7 +2046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P172" authorId="2">
+    <comment ref="P172" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000055000000}">
       <text>
         <r>
           <rPr>
@@ -2064,7 +2070,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P173" authorId="2">
+    <comment ref="P173" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000056000000}">
       <text>
         <r>
           <rPr>
@@ -2088,7 +2094,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L174" authorId="2">
+    <comment ref="L174" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000057000000}">
       <text>
         <r>
           <rPr>
@@ -2112,7 +2118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ183" authorId="0">
+    <comment ref="AQ183" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000058000000}">
       <text>
         <r>
           <rPr>
@@ -2136,7 +2142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA204" authorId="1">
+    <comment ref="AA204" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000059000000}">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB204" authorId="1">
+    <comment ref="AB204" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005A000000}">
       <text>
         <r>
           <rPr>
@@ -2184,7 +2190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC204" authorId="1">
+    <comment ref="AC204" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005B000000}">
       <text>
         <r>
           <rPr>
@@ -2208,7 +2214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P207" authorId="2">
+    <comment ref="P207" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005C000000}">
       <text>
         <r>
           <rPr>
@@ -2232,7 +2238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P208" authorId="2">
+    <comment ref="P208" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005D000000}">
       <text>
         <r>
           <rPr>
@@ -2256,7 +2262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P209" authorId="2">
+    <comment ref="P209" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005E000000}">
       <text>
         <r>
           <rPr>
@@ -2280,7 +2286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P210" authorId="2">
+    <comment ref="P210" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005F000000}">
       <text>
         <r>
           <rPr>
@@ -2304,7 +2310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P211" authorId="2">
+    <comment ref="P211" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000060000000}">
       <text>
         <r>
           <rPr>
@@ -2328,7 +2334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P212" authorId="2">
+    <comment ref="P212" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000061000000}">
       <text>
         <r>
           <rPr>
@@ -2352,7 +2358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P228" authorId="2">
+    <comment ref="P228" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000062000000}">
       <text>
         <r>
           <rPr>
@@ -2376,7 +2382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P229" authorId="2">
+    <comment ref="P229" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000063000000}">
       <text>
         <r>
           <rPr>
@@ -2400,7 +2406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P230" authorId="2">
+    <comment ref="P230" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000064000000}">
       <text>
         <r>
           <rPr>
@@ -2424,7 +2430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P231" authorId="2">
+    <comment ref="P231" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000065000000}">
       <text>
         <r>
           <rPr>
@@ -2448,7 +2454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P232" authorId="2">
+    <comment ref="P232" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000066000000}">
       <text>
         <r>
           <rPr>
@@ -2472,7 +2478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P233" authorId="2">
+    <comment ref="P233" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000067000000}">
       <text>
         <r>
           <rPr>
@@ -2496,7 +2502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P234" authorId="2">
+    <comment ref="P234" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000068000000}">
       <text>
         <r>
           <rPr>
@@ -2520,7 +2526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P235" authorId="2">
+    <comment ref="P235" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000069000000}">
       <text>
         <r>
           <rPr>
@@ -2544,7 +2550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P236" authorId="2">
+    <comment ref="P236" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006A000000}">
       <text>
         <r>
           <rPr>
@@ -2568,7 +2574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P237" authorId="2">
+    <comment ref="P237" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006B000000}">
       <text>
         <r>
           <rPr>
@@ -2592,7 +2598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P238" authorId="2">
+    <comment ref="P238" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006C000000}">
       <text>
         <r>
           <rPr>
@@ -2616,7 +2622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P239" authorId="2">
+    <comment ref="P239" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006D000000}">
       <text>
         <r>
           <rPr>
@@ -2640,7 +2646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P240" authorId="2">
+    <comment ref="P240" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006E000000}">
       <text>
         <r>
           <rPr>
@@ -2664,7 +2670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P241" authorId="2">
+    <comment ref="P241" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006F000000}">
       <text>
         <r>
           <rPr>
@@ -2688,7 +2694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P242" authorId="2">
+    <comment ref="P242" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000070000000}">
       <text>
         <r>
           <rPr>
@@ -2712,7 +2718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P243" authorId="2">
+    <comment ref="P243" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000071000000}">
       <text>
         <r>
           <rPr>
@@ -2736,7 +2742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P244" authorId="2">
+    <comment ref="P244" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000072000000}">
       <text>
         <r>
           <rPr>
@@ -2760,7 +2766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P245" authorId="2">
+    <comment ref="P245" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000073000000}">
       <text>
         <r>
           <rPr>
@@ -2784,7 +2790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P246" authorId="2">
+    <comment ref="P246" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000074000000}">
       <text>
         <r>
           <rPr>
@@ -2808,7 +2814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA246" authorId="1">
+    <comment ref="AA246" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000075000000}">
       <text>
         <r>
           <rPr>
@@ -2832,7 +2838,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P247" authorId="2">
+    <comment ref="P247" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000076000000}">
       <text>
         <r>
           <rPr>
@@ -2856,7 +2862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P248" authorId="2">
+    <comment ref="P248" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000077000000}">
       <text>
         <r>
           <rPr>
@@ -2880,7 +2886,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P249" authorId="2">
+    <comment ref="P249" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000078000000}">
       <text>
         <r>
           <rPr>
@@ -2904,7 +2910,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P250" authorId="2">
+    <comment ref="P250" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000079000000}">
       <text>
         <r>
           <rPr>
@@ -2928,7 +2934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P251" authorId="2">
+    <comment ref="P251" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007A000000}">
       <text>
         <r>
           <rPr>
@@ -2952,7 +2958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL251" authorId="1">
+    <comment ref="AL251" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007B000000}">
       <text>
         <r>
           <rPr>
@@ -2976,7 +2982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P252" authorId="2">
+    <comment ref="P252" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007C000000}">
       <text>
         <r>
           <rPr>
@@ -3000,7 +3006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P253" authorId="2">
+    <comment ref="P253" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007D000000}">
       <text>
         <r>
           <rPr>
@@ -3024,7 +3030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P254" authorId="2">
+    <comment ref="P254" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007E000000}">
       <text>
         <r>
           <rPr>
@@ -3048,7 +3054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P255" authorId="2">
+    <comment ref="P255" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00007F000000}">
       <text>
         <r>
           <rPr>
@@ -3072,7 +3078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P256" authorId="2">
+    <comment ref="P256" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000080000000}">
       <text>
         <r>
           <rPr>
@@ -3096,7 +3102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P257" authorId="2">
+    <comment ref="P257" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000081000000}">
       <text>
         <r>
           <rPr>
@@ -3120,7 +3126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P258" authorId="2">
+    <comment ref="P258" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000082000000}">
       <text>
         <r>
           <rPr>
@@ -3144,7 +3150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P259" authorId="2">
+    <comment ref="P259" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000083000000}">
       <text>
         <r>
           <rPr>
@@ -3168,7 +3174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W259" authorId="0">
+    <comment ref="W259" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000084000000}">
       <text>
         <r>
           <rPr>
@@ -3192,7 +3198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P260" authorId="2">
+    <comment ref="P260" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000085000000}">
       <text>
         <r>
           <rPr>
@@ -3216,7 +3222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P261" authorId="2">
+    <comment ref="P261" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000086000000}">
       <text>
         <r>
           <rPr>
@@ -3240,7 +3246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P262" authorId="2">
+    <comment ref="P262" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000087000000}">
       <text>
         <r>
           <rPr>
@@ -3264,7 +3270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P263" authorId="2">
+    <comment ref="P263" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000088000000}">
       <text>
         <r>
           <rPr>
@@ -3288,7 +3294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P264" authorId="2">
+    <comment ref="P264" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000089000000}">
       <text>
         <r>
           <rPr>
@@ -3312,7 +3318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P265" authorId="2">
+    <comment ref="P265" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008A000000}">
       <text>
         <r>
           <rPr>
@@ -3336,7 +3342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P266" authorId="2">
+    <comment ref="P266" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008B000000}">
       <text>
         <r>
           <rPr>
@@ -3360,7 +3366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P267" authorId="2">
+    <comment ref="P267" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008C000000}">
       <text>
         <r>
           <rPr>
@@ -3384,7 +3390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P268" authorId="2">
+    <comment ref="P268" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008D000000}">
       <text>
         <r>
           <rPr>
@@ -3408,7 +3414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W268" authorId="0">
+    <comment ref="W268" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008E000000}">
       <text>
         <r>
           <rPr>
@@ -3432,7 +3438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z268" authorId="0">
+    <comment ref="Z268" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00008F000000}">
       <text>
         <r>
           <rPr>
@@ -3456,7 +3462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I269" authorId="2">
+    <comment ref="I269" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000090000000}">
       <text>
         <r>
           <rPr>
@@ -3480,7 +3486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P269" authorId="2">
+    <comment ref="P269" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000091000000}">
       <text>
         <r>
           <rPr>
@@ -3504,7 +3510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P270" authorId="2">
+    <comment ref="P270" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000092000000}">
       <text>
         <r>
           <rPr>
@@ -3528,7 +3534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P271" authorId="2">
+    <comment ref="P271" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000093000000}">
       <text>
         <r>
           <rPr>
@@ -3552,7 +3558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V277" authorId="0">
+    <comment ref="V277" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000094000000}">
       <text>
         <r>
           <rPr>
@@ -3576,7 +3582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W286" authorId="0">
+    <comment ref="W286" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000095000000}">
       <text>
         <r>
           <rPr>
@@ -3600,7 +3606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z286" authorId="0">
+    <comment ref="Z286" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000096000000}">
       <text>
         <r>
           <rPr>
@@ -3624,7 +3630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S288" authorId="0">
+    <comment ref="S288" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000097000000}">
       <text>
         <r>
           <rPr>
@@ -3648,7 +3654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W288" authorId="0">
+    <comment ref="W288" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000098000000}">
       <text>
         <r>
           <rPr>
@@ -3672,7 +3678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W289" authorId="0">
+    <comment ref="W289" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000099000000}">
       <text>
         <r>
           <rPr>
@@ -3696,7 +3702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z289" authorId="0">
+    <comment ref="Z289" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00009A000000}">
       <text>
         <r>
           <rPr>
@@ -9007,7 +9013,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
@@ -9913,48 +9919,48 @@
     <xf numFmtId="164" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="3" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="4" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="5" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="6" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="7" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9967,14 +9973,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -10012,9 +10021,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10047,9 +10056,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10082,9 +10108,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -10257,74 +10300,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AX305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="Z65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="P85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE75" sqref="AE75"/>
+      <selection pane="bottomRight" activeCell="V94" sqref="V94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="10" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" style="1" customWidth="1"/>
     <col min="25" max="25" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6" style="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" style="1" customWidth="1"/>
     <col min="30" max="30" width="19" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.85546875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="17.140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="16.5703125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="16.140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="13.85546875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="11.7109375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="26.140625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.28515625" style="29" customWidth="1"/>
-    <col min="42" max="42" width="19.28515625" style="51" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="16.5" style="1" customWidth="1"/>
+    <col min="35" max="35" width="16.1640625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="13.83203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="11.6640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="26.1640625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.33203125" style="29" customWidth="1"/>
+    <col min="42" max="42" width="19.33203125" style="51" customWidth="1"/>
     <col min="43" max="43" width="18" style="1" customWidth="1"/>
-    <col min="44" max="44" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.7109375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.6640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="29" style="1" customWidth="1"/>
-    <col min="50" max="50" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="9.140625" style="1"/>
+    <col min="50" max="50" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>1541</v>
       </c>
@@ -10476,7 +10519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -10619,7 +10662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -10759,7 +10802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -10905,7 +10948,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="5" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -11048,7 +11091,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="6" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -11188,7 +11231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="78">
         <v>6</v>
       </c>
@@ -11280,7 +11323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -11420,7 +11463,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -11556,7 +11599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -11698,7 +11741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -11844,7 +11887,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -11990,7 +12033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -12132,7 +12175,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -12275,7 +12318,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -12421,7 +12464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -12567,7 +12610,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -12706,7 +12749,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -12848,7 +12891,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -12990,7 +13033,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -13132,7 +13175,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -13274,7 +13317,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -13416,7 +13459,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="23" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -13558,7 +13601,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -13697,7 +13740,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -13839,7 +13882,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -13981,7 +14024,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -14123,7 +14166,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -14215,7 +14258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -14310,7 +14353,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="30" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -14405,7 +14448,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="31" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -14497,7 +14540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="78">
         <v>31</v>
       </c>
@@ -14592,7 +14635,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="33" spans="1:50" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -14733,7 +14776,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="34" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -14879,7 +14922,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -15025,7 +15068,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -15171,7 +15214,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -15317,7 +15360,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -15463,7 +15506,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -15558,7 +15601,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="40" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -15650,7 +15693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -15742,7 +15785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -15834,7 +15877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="78">
         <v>42</v>
       </c>
@@ -15926,7 +15969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -16072,7 +16115,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -16167,7 +16210,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="46" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -16254,7 +16297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="78">
         <v>46</v>
       </c>
@@ -16344,7 +16387,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="48" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -16496,7 +16539,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -16594,7 +16637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -16719,7 +16762,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="51" spans="1:50" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" s="87" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="87">
         <v>50</v>
       </c>
@@ -16798,7 +16841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:50" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" s="4" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -16944,7 +16987,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -17087,7 +17130,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -17176,7 +17219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="78">
         <v>54</v>
       </c>
@@ -17265,7 +17308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -17408,7 +17451,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -17497,7 +17540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -17640,7 +17683,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="59" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -17786,7 +17829,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="60" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -17932,7 +17975,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="61" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -18078,7 +18121,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="62" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>61</v>
       </c>
@@ -18224,7 +18267,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="63" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -18365,7 +18408,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="64" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -18503,7 +18546,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="65" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -18641,7 +18684,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="66" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -18730,7 +18773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -18819,7 +18862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -18908,7 +18951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -18997,7 +19040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -19089,7 +19132,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="71" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -19241,7 +19284,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="72" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -19393,7 +19436,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="73" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -19542,7 +19585,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="74" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -19694,7 +19737,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="75" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -19841,7 +19884,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="76" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -19990,7 +20033,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="77" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -20088,7 +20131,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="78" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -20183,7 +20226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -20278,7 +20321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -20373,7 +20416,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="19">
         <v>80</v>
       </c>
@@ -20468,7 +20511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -20614,7 +20657,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="83" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -20760,7 +20803,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="84" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -20906,7 +20949,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="85" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -21052,7 +21095,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="86" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -21198,7 +21241,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="87" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -21287,7 +21330,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -21376,7 +21419,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -21465,7 +21508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -21554,7 +21597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="19">
         <v>90</v>
       </c>
@@ -21643,7 +21686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -21786,7 +21829,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="93" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -21929,7 +21972,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="94" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -21987,8 +22030,8 @@
       <c r="U94" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V94" s="4" t="s">
-        <v>165</v>
+      <c r="V94" s="257" t="s">
+        <v>8</v>
       </c>
       <c r="W94" s="4" t="s">
         <v>19</v>
@@ -22075,7 +22118,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="95" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -22218,7 +22261,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="96" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -22360,7 +22403,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="97" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -22506,7 +22549,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="98" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -22648,7 +22691,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="99" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -22737,7 +22780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -22826,7 +22869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -22915,7 +22958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -23004,7 +23047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="19">
         <v>102</v>
       </c>
@@ -23093,7 +23136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -23245,7 +23288,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="105" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -23394,7 +23437,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -23543,7 +23586,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="107" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -23641,7 +23684,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="108" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -23736,7 +23779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="19">
         <v>108</v>
       </c>
@@ -23831,7 +23874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -23983,7 +24026,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="111" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -24132,7 +24175,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="112" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -24284,7 +24327,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="113" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -24432,7 +24475,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="114" spans="1:50" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:50" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="43">
         <v>297</v>
       </c>
@@ -24576,7 +24619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>113</v>
       </c>
@@ -24724,7 +24767,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="116" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>114</v>
       </c>
@@ -24876,7 +24919,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="117" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>115</v>
       </c>
@@ -25025,7 +25068,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="118" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>116</v>
       </c>
@@ -25170,7 +25213,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="119" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>117</v>
       </c>
@@ -25315,7 +25358,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="120" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>118</v>
       </c>
@@ -25463,7 +25506,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="121" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>119</v>
       </c>
@@ -25558,7 +25601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>120</v>
       </c>
@@ -25653,7 +25696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>121</v>
       </c>
@@ -25748,7 +25791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>122</v>
       </c>
@@ -25843,7 +25886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="19">
         <v>123</v>
       </c>
@@ -25938,7 +25981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>124</v>
       </c>
@@ -26081,7 +26124,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="127" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>125</v>
       </c>
@@ -26224,7 +26267,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="128" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>126</v>
       </c>
@@ -26366,7 +26409,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="129" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>127</v>
       </c>
@@ -26512,7 +26555,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="130" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>128</v>
       </c>
@@ -26658,7 +26701,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="131" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>129</v>
       </c>
@@ -26804,7 +26847,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="132" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>130</v>
       </c>
@@ -26893,7 +26936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>131</v>
       </c>
@@ -26982,7 +27025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>132</v>
       </c>
@@ -27071,7 +27114,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>133</v>
       </c>
@@ -27160,7 +27203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="136" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="19">
         <v>134</v>
       </c>
@@ -27249,7 +27292,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>135</v>
       </c>
@@ -27392,7 +27435,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="138" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>136</v>
       </c>
@@ -27535,7 +27578,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="139" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>137</v>
       </c>
@@ -27678,7 +27721,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="140" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>138</v>
       </c>
@@ -27824,7 +27867,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="141" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>139</v>
       </c>
@@ -27913,7 +27956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>140</v>
       </c>
@@ -28002,7 +28045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>141</v>
       </c>
@@ -28091,7 +28134,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="19">
         <v>142</v>
       </c>
@@ -28183,7 +28226,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="145" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>143</v>
       </c>
@@ -28335,7 +28378,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="146" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>144</v>
       </c>
@@ -28487,7 +28530,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="147" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>145</v>
       </c>
@@ -28639,7 +28682,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="148" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>146</v>
       </c>
@@ -28788,7 +28831,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="149" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>147</v>
       </c>
@@ -28883,7 +28926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>148</v>
       </c>
@@ -28978,7 +29021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:50" s="177" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:50" s="177" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="177">
         <v>149</v>
       </c>
@@ -29076,7 +29119,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="152" spans="1:50" s="180" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:50" s="180" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="180">
         <v>150</v>
       </c>
@@ -29171,7 +29214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>151</v>
       </c>
@@ -29323,7 +29366,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="154" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>152</v>
       </c>
@@ -29472,7 +29515,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="155" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>153</v>
       </c>
@@ -29624,7 +29667,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="156" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
         <v>154</v>
       </c>
@@ -29770,7 +29813,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="157" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
         <v>155</v>
       </c>
@@ -29916,7 +29959,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="158" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
         <v>156</v>
       </c>
@@ -30062,7 +30105,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="159" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>157</v>
       </c>
@@ -30160,7 +30203,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="160" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
         <v>158</v>
       </c>
@@ -30258,7 +30301,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="161" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>159</v>
       </c>
@@ -30350,7 +30393,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="162" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>160</v>
       </c>
@@ -30442,7 +30485,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="163" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="19">
         <v>161</v>
       </c>
@@ -30534,7 +30577,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="164" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>162</v>
       </c>
@@ -30686,7 +30729,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="165" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>163</v>
       </c>
@@ -30835,7 +30878,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="166" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>164</v>
       </c>
@@ -30984,7 +31027,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="167" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>165</v>
       </c>
@@ -31136,7 +31179,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="168" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>166</v>
       </c>
@@ -31285,7 +31328,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="169" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>167</v>
       </c>
@@ -31380,7 +31423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>168</v>
       </c>
@@ -31475,7 +31518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>169</v>
       </c>
@@ -31570,7 +31613,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="172" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>170</v>
       </c>
@@ -31665,7 +31708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="19">
         <v>171</v>
       </c>
@@ -31760,7 +31803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>172</v>
       </c>
@@ -31903,7 +31946,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="175" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
         <v>173</v>
       </c>
@@ -32049,7 +32092,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="176" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>174</v>
       </c>
@@ -32141,7 +32184,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="177" spans="1:50" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:50" s="87" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="87">
         <v>175</v>
       </c>
@@ -32230,7 +32273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:50" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:50" s="4" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>176</v>
       </c>
@@ -32373,7 +32416,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="179" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>177</v>
       </c>
@@ -32516,7 +32559,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="180" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>178</v>
       </c>
@@ -32608,7 +32651,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="181" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="19">
         <v>179</v>
       </c>
@@ -32697,7 +32740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
         <v>180</v>
       </c>
@@ -32843,7 +32886,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="183" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
         <v>181</v>
       </c>
@@ -32989,7 +33032,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="184" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
         <v>182</v>
       </c>
@@ -33135,7 +33178,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="185" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
         <v>183</v>
       </c>
@@ -33224,7 +33267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
         <v>184</v>
       </c>
@@ -33313,7 +33356,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="19">
         <v>185</v>
       </c>
@@ -33402,7 +33445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
         <v>186</v>
       </c>
@@ -33545,7 +33588,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="189" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
         <v>187</v>
       </c>
@@ -33691,7 +33734,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="190" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="4">
         <v>188</v>
       </c>
@@ -33837,7 +33880,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="191" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>189</v>
       </c>
@@ -33983,7 +34026,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="192" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="4">
         <v>190</v>
       </c>
@@ -34126,7 +34169,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="193" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
         <v>191</v>
       </c>
@@ -34215,7 +34258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="4">
         <v>192</v>
       </c>
@@ -34304,7 +34347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
         <v>193</v>
       </c>
@@ -34393,7 +34436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>194</v>
       </c>
@@ -34482,7 +34525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="19">
         <v>195</v>
       </c>
@@ -34571,7 +34614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
         <v>196</v>
       </c>
@@ -34717,7 +34760,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="199" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
         <v>197</v>
       </c>
@@ -34863,7 +34906,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="200" spans="1:50" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:50" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="25">
         <v>296</v>
       </c>
@@ -35000,7 +35043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
         <v>198</v>
       </c>
@@ -35146,7 +35189,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="202" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
         <v>199</v>
       </c>
@@ -35235,7 +35278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="203" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
         <v>200</v>
       </c>
@@ -35322,7 +35365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="204" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
         <v>201</v>
       </c>
@@ -35434,7 +35477,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="205" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="4">
         <v>202</v>
       </c>
@@ -35523,7 +35566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="206" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="19">
         <v>203</v>
       </c>
@@ -35612,7 +35655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="4">
         <v>204</v>
       </c>
@@ -35764,7 +35807,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="208" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="4">
         <v>205</v>
       </c>
@@ -35916,7 +35959,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="209" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="4">
         <v>206</v>
       </c>
@@ -36068,7 +36111,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="210" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="4">
         <v>207</v>
       </c>
@@ -36166,7 +36209,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="211" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="4">
         <v>208</v>
       </c>
@@ -36261,7 +36304,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="19">
         <v>209</v>
       </c>
@@ -36356,7 +36399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="4">
         <v>210</v>
       </c>
@@ -36499,7 +36542,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="214" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="4">
         <v>211</v>
       </c>
@@ -36641,7 +36684,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="215" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="4">
         <v>212</v>
       </c>
@@ -36787,7 +36830,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="216" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="4">
         <v>213</v>
       </c>
@@ -36930,7 +36973,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="217" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="4">
         <v>214</v>
       </c>
@@ -37073,7 +37116,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="218" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="4">
         <v>215</v>
       </c>
@@ -37212,7 +37255,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="219" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="4">
         <v>216</v>
       </c>
@@ -37358,7 +37401,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="220" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="4">
         <v>217</v>
       </c>
@@ -37497,7 +37540,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="221" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="4">
         <v>218</v>
       </c>
@@ -37636,7 +37679,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="222" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="4">
         <v>219</v>
       </c>
@@ -37775,7 +37818,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="223" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="4">
         <v>220</v>
       </c>
@@ -37864,7 +37907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="4">
         <v>221</v>
       </c>
@@ -37956,7 +37999,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="225" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
         <v>222</v>
       </c>
@@ -38045,7 +38088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="226" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="4">
         <v>223</v>
       </c>
@@ -38134,7 +38177,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="19">
         <v>224</v>
       </c>
@@ -38223,7 +38266,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="228" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="4">
         <v>225</v>
       </c>
@@ -38372,7 +38415,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="229" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="4">
         <v>226</v>
       </c>
@@ -38521,7 +38564,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="230" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230" s="4">
         <v>227</v>
       </c>
@@ -38670,7 +38713,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="231" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231" s="4">
         <v>228</v>
       </c>
@@ -38765,7 +38808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="232" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A232" s="4">
         <v>229</v>
       </c>
@@ -38860,7 +38903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A233" s="19">
         <v>230</v>
       </c>
@@ -38955,7 +38998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="234" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A234" s="4">
         <v>231</v>
       </c>
@@ -39107,7 +39150,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="235" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A235" s="4">
         <v>232</v>
       </c>
@@ -39256,7 +39299,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="236" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A236" s="4">
         <v>233</v>
       </c>
@@ -39408,7 +39451,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="237" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237" s="4">
         <v>234</v>
       </c>
@@ -39560,7 +39603,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="238" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="4">
         <v>235</v>
       </c>
@@ -39709,7 +39752,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="239" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="4">
         <v>236</v>
       </c>
@@ -39854,7 +39897,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="240" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240" s="4">
         <v>237</v>
       </c>
@@ -40002,7 +40045,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="241" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A241" s="4">
         <v>238</v>
       </c>
@@ -40100,7 +40143,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="242" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A242" s="4">
         <v>239</v>
       </c>
@@ -40195,7 +40238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="243" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" s="4">
         <v>240</v>
       </c>
@@ -40293,7 +40336,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="244" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244" s="4">
         <v>241</v>
       </c>
@@ -40388,7 +40431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="245" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" s="19">
         <v>242</v>
       </c>
@@ -40483,7 +40526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="246" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A246" s="4">
         <v>243</v>
       </c>
@@ -40633,7 +40676,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="247" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" s="4">
         <v>244</v>
       </c>
@@ -40782,7 +40825,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="248" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A248" s="4">
         <v>245</v>
       </c>
@@ -40931,7 +40974,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="249" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="4">
         <v>246</v>
       </c>
@@ -41083,7 +41126,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="250" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250" s="4">
         <v>247</v>
       </c>
@@ -41232,7 +41275,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="251" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251" s="4">
         <v>248</v>
       </c>
@@ -41380,7 +41423,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="252" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A252" s="4">
         <v>249</v>
       </c>
@@ -41528,7 +41571,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="253" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253" s="4">
         <v>250</v>
       </c>
@@ -41621,7 +41664,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="254" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A254" s="4">
         <v>251</v>
       </c>
@@ -41716,7 +41759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255" s="4">
         <v>252</v>
       </c>
@@ -41811,7 +41854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A256" s="4">
         <v>253</v>
       </c>
@@ -41906,7 +41949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="257" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="19">
         <v>254</v>
       </c>
@@ -42001,7 +42044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" s="4">
         <v>255</v>
       </c>
@@ -42150,7 +42193,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="259" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A259" s="4">
         <v>256</v>
       </c>
@@ -42302,7 +42345,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="260" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A260" s="4">
         <v>257</v>
       </c>
@@ -42451,7 +42494,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="261" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="4">
         <v>258</v>
       </c>
@@ -42600,7 +42643,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="262" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262" s="4">
         <v>259</v>
       </c>
@@ -42695,7 +42738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A263" s="4">
         <v>260</v>
       </c>
@@ -42790,7 +42833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264" s="4">
         <v>261</v>
       </c>
@@ -42885,7 +42928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="265" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A265" s="19">
         <v>262</v>
       </c>
@@ -42980,7 +43023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A266" s="4">
         <v>263</v>
       </c>
@@ -43132,7 +43175,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="267" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A267" s="4">
         <v>264</v>
       </c>
@@ -43284,7 +43327,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="268" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268" s="4">
         <v>265</v>
       </c>
@@ -43436,7 +43479,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="269" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A269" s="4">
         <v>266</v>
       </c>
@@ -43534,7 +43577,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="270" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A270" s="4">
         <v>267</v>
       </c>
@@ -43629,7 +43672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="271" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A271" s="19">
         <v>268</v>
       </c>
@@ -43724,7 +43767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="272" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272" s="4">
         <v>269</v>
       </c>
@@ -43867,7 +43910,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="273" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A273" s="4">
         <v>270</v>
       </c>
@@ -44010,7 +44053,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="274" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A274" s="4">
         <v>271</v>
       </c>
@@ -44149,7 +44192,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="275" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A275" s="4">
         <v>272</v>
       </c>
@@ -44292,7 +44335,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="276" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A276" s="4">
         <v>273</v>
       </c>
@@ -44435,7 +44478,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="277" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A277" s="4">
         <v>274</v>
       </c>
@@ -44581,7 +44624,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="278" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A278" s="4">
         <v>275</v>
       </c>
@@ -44720,7 +44763,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="279" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A279" s="4">
         <v>276</v>
       </c>
@@ -44862,7 +44905,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="280" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A280" s="4">
         <v>277</v>
       </c>
@@ -44951,7 +44994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="281" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A281" s="4">
         <v>278</v>
       </c>
@@ -45040,7 +45083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="282" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A282" s="4">
         <v>279</v>
       </c>
@@ -45129,7 +45172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A283" s="4">
         <v>280</v>
       </c>
@@ -45218,7 +45261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="284" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A284" s="19">
         <v>281</v>
       </c>
@@ -45307,7 +45350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="285" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A285" s="4">
         <v>282</v>
       </c>
@@ -45445,7 +45488,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="286" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A286" s="4">
         <v>283</v>
       </c>
@@ -45588,7 +45631,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="287" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A287" s="4">
         <v>284</v>
       </c>
@@ -45731,7 +45774,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="288" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A288" s="4">
         <v>285</v>
       </c>
@@ -45877,7 +45920,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="289" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289" s="4">
         <v>286</v>
       </c>
@@ -46020,7 +46063,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="290" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290" s="4">
         <v>287</v>
       </c>
@@ -46162,7 +46205,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="291" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="4">
         <v>288</v>
       </c>
@@ -46304,7 +46347,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="292" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A292" s="4">
         <v>289</v>
       </c>
@@ -46446,7 +46489,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="293" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293" s="4">
         <v>290</v>
       </c>
@@ -46589,7 +46632,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="294" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294" s="4">
         <v>291</v>
       </c>
@@ -46678,7 +46721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="295" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295" s="4">
         <v>292</v>
       </c>
@@ -46767,7 +46810,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="296" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296" s="4">
         <v>293</v>
       </c>
@@ -46856,7 +46899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="297" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A297" s="4">
         <v>294</v>
       </c>
@@ -46945,7 +46988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="298" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298" s="4">
         <v>295</v>
       </c>
@@ -47034,43 +47077,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="299" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H299" s="1"/>
       <c r="Q299" s="2"/>
       <c r="AO299" s="50"/>
       <c r="AP299" s="50"/>
     </row>
-    <row r="300" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H300" s="1"/>
       <c r="Q300" s="2"/>
       <c r="AO300" s="50"/>
       <c r="AP300" s="50"/>
     </row>
-    <row r="301" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H301" s="1"/>
       <c r="Q301" s="2"/>
       <c r="AO301" s="50"/>
       <c r="AP301" s="50"/>
     </row>
-    <row r="302" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H302" s="1"/>
       <c r="Q302" s="2"/>
       <c r="AO302" s="50"/>
       <c r="AP302" s="50"/>
     </row>
-    <row r="303" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H303" s="1"/>
       <c r="Q303" s="2"/>
       <c r="AO303" s="28"/>
       <c r="AP303" s="50"/>
     </row>
-    <row r="304" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H304" s="1"/>
       <c r="Q304" s="3"/>
       <c r="AO304" s="28"/>
       <c r="AP304" s="50"/>
     </row>
-    <row r="305" spans="8:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="8:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H305" s="1"/>
       <c r="Q305" s="3"/>
       <c r="AO305" s="28"/>

</xml_diff>